<commit_message>
change so that everything can be commited to github
</commit_message>
<xml_diff>
--- a/input/Book1a.xlsx
+++ b/input/Book1a.xlsx
@@ -3,22 +3,31 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <workbookProtection workbookPassword="CBEB" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7485"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7485" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Evaluation Warning" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <definedNames/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>Evaluation Only. Created with Aspose.Cells for Java.Copyright 2003 - 2016 Aspose Pty Ltd.</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -26,10 +35,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="18"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -44,17 +66,115 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment/>
+      <protection/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0"/>
+    <cellStyle name="Percent" xfId="15"/>
+    <cellStyle name="Currency" xfId="16"/>
+    <cellStyle name="Currency [0]" xfId="17"/>
+    <cellStyle name="Comma" xfId="18"/>
+    <cellStyle name="Comma [0]" xfId="19"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -349,37 +469,63 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0" topLeftCell="A1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+  <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" topLeftCell="A1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+  <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" topLeftCell="A1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <dimension ref="A5:A5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetData>
+    <row r="5" ht="23.25" customHeight="1">
+      <c r="A5" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait"/>
+  <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>